<commit_message>
edit dataset and build apps
</commit_message>
<xml_diff>
--- a/telur_clean.xlsx
+++ b/telur_clean.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,15 +436,20 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>pixel</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>volume</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>jarak</t>
         </is>
@@ -455,12 +460,15 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
         <v>57378</v>
       </c>
-      <c r="C2" t="n">
-        <v>5.999999999999999e-05</v>
-      </c>
       <c r="D2" t="n">
+        <v>59.99999999999999</v>
+      </c>
+      <c r="E2" t="n">
         <v>0.307</v>
       </c>
     </row>
@@ -469,12 +477,15 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
         <v>53078</v>
       </c>
-      <c r="C3" t="n">
-        <v>5e-05</v>
-      </c>
       <c r="D3" t="n">
+        <v>50</v>
+      </c>
+      <c r="E3" t="n">
         <v>0.307</v>
       </c>
     </row>
@@ -483,12 +494,15 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="n">
         <v>60613</v>
       </c>
-      <c r="C4" t="n">
-        <v>5.999999999999999e-05</v>
-      </c>
       <c r="D4" t="n">
+        <v>59.99999999999999</v>
+      </c>
+      <c r="E4" t="n">
         <v>0.307</v>
       </c>
     </row>
@@ -497,12 +511,15 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="n">
         <v>53295</v>
       </c>
-      <c r="C5" t="n">
-        <v>5e-05</v>
-      </c>
       <c r="D5" t="n">
+        <v>50</v>
+      </c>
+      <c r="E5" t="n">
         <v>0.307</v>
       </c>
     </row>
@@ -511,12 +528,15 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="n">
         <v>44062</v>
       </c>
-      <c r="C6" t="n">
-        <v>4e-05</v>
-      </c>
       <c r="D6" t="n">
+        <v>40</v>
+      </c>
+      <c r="E6" t="n">
         <v>0.307</v>
       </c>
     </row>
@@ -525,12 +545,15 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" t="n">
         <v>47379</v>
       </c>
-      <c r="C7" t="n">
-        <v>4.5e-05</v>
-      </c>
       <c r="D7" t="n">
+        <v>45</v>
+      </c>
+      <c r="E7" t="n">
         <v>0.307</v>
       </c>
     </row>
@@ -539,12 +562,15 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" t="n">
         <v>58702</v>
       </c>
-      <c r="C8" t="n">
-        <v>5.999999999999999e-05</v>
-      </c>
       <c r="D8" t="n">
+        <v>59.99999999999999</v>
+      </c>
+      <c r="E8" t="n">
         <v>0.307</v>
       </c>
     </row>
@@ -553,12 +579,15 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
+        <v>7</v>
+      </c>
+      <c r="C9" t="n">
         <v>44331</v>
       </c>
-      <c r="C9" t="n">
-        <v>4.5e-05</v>
-      </c>
       <c r="D9" t="n">
+        <v>45</v>
+      </c>
+      <c r="E9" t="n">
         <v>0.307</v>
       </c>
     </row>
@@ -567,12 +596,15 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
+        <v>8</v>
+      </c>
+      <c r="C10" t="n">
         <v>56897</v>
       </c>
-      <c r="C10" t="n">
-        <v>5.5e-05</v>
-      </c>
       <c r="D10" t="n">
+        <v>55</v>
+      </c>
+      <c r="E10" t="n">
         <v>0.307</v>
       </c>
     </row>
@@ -581,12 +613,15 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
+        <v>9</v>
+      </c>
+      <c r="C11" t="n">
         <v>44617</v>
       </c>
-      <c r="C11" t="n">
-        <v>4e-05</v>
-      </c>
       <c r="D11" t="n">
+        <v>40</v>
+      </c>
+      <c r="E11" t="n">
         <v>0.307</v>
       </c>
     </row>
@@ -595,12 +630,15 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
+        <v>10</v>
+      </c>
+      <c r="C12" t="n">
         <v>58183</v>
       </c>
-      <c r="C12" t="n">
-        <v>5.5e-05</v>
-      </c>
       <c r="D12" t="n">
+        <v>55</v>
+      </c>
+      <c r="E12" t="n">
         <v>0.307</v>
       </c>
     </row>
@@ -609,12 +647,15 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
+        <v>11</v>
+      </c>
+      <c r="C13" t="n">
         <v>56427</v>
       </c>
-      <c r="C13" t="n">
-        <v>5.999999999999999e-05</v>
-      </c>
       <c r="D13" t="n">
+        <v>59.99999999999999</v>
+      </c>
+      <c r="E13" t="n">
         <v>0.307</v>
       </c>
     </row>
@@ -623,12 +664,15 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
+        <v>12</v>
+      </c>
+      <c r="C14" t="n">
         <v>58838</v>
       </c>
-      <c r="C14" t="n">
-        <v>5.999999999999999e-05</v>
-      </c>
       <c r="D14" t="n">
+        <v>59.99999999999999</v>
+      </c>
+      <c r="E14" t="n">
         <v>0.307</v>
       </c>
     </row>
@@ -637,12 +681,15 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
+        <v>13</v>
+      </c>
+      <c r="C15" t="n">
         <v>66614</v>
       </c>
-      <c r="C15" t="n">
-        <v>7.499999999999999e-05</v>
-      </c>
       <c r="D15" t="n">
+        <v>75</v>
+      </c>
+      <c r="E15" t="n">
         <v>0.307</v>
       </c>
     </row>
@@ -651,12 +698,15 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
+        <v>14</v>
+      </c>
+      <c r="C16" t="n">
         <v>60512</v>
       </c>
-      <c r="C16" t="n">
-        <v>5.999999999999999e-05</v>
-      </c>
       <c r="D16" t="n">
+        <v>59.99999999999999</v>
+      </c>
+      <c r="E16" t="n">
         <v>0.307</v>
       </c>
     </row>
@@ -665,12 +715,15 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
+        <v>15</v>
+      </c>
+      <c r="C17" t="n">
         <v>57192</v>
       </c>
-      <c r="C17" t="n">
-        <v>5.999999999999999e-05</v>
-      </c>
       <c r="D17" t="n">
+        <v>59.99999999999999</v>
+      </c>
+      <c r="E17" t="n">
         <v>0.307</v>
       </c>
     </row>
@@ -679,12 +732,15 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
+        <v>16</v>
+      </c>
+      <c r="C18" t="n">
         <v>54665</v>
       </c>
-      <c r="C18" t="n">
-        <v>5.5e-05</v>
-      </c>
       <c r="D18" t="n">
+        <v>55</v>
+      </c>
+      <c r="E18" t="n">
         <v>0.307</v>
       </c>
     </row>
@@ -693,12 +749,15 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
+        <v>17</v>
+      </c>
+      <c r="C19" t="n">
         <v>60386</v>
       </c>
-      <c r="C19" t="n">
-        <v>6.499999999999999e-05</v>
-      </c>
       <c r="D19" t="n">
+        <v>65</v>
+      </c>
+      <c r="E19" t="n">
         <v>0.307</v>
       </c>
     </row>
@@ -707,12 +766,15 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
+        <v>18</v>
+      </c>
+      <c r="C20" t="n">
         <v>44675</v>
       </c>
-      <c r="C20" t="n">
-        <v>4e-05</v>
-      </c>
       <c r="D20" t="n">
+        <v>40</v>
+      </c>
+      <c r="E20" t="n">
         <v>0.307</v>
       </c>
     </row>
@@ -721,12 +783,15 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
+        <v>19</v>
+      </c>
+      <c r="C21" t="n">
         <v>51767</v>
       </c>
-      <c r="C21" t="n">
-        <v>5e-05</v>
-      </c>
       <c r="D21" t="n">
+        <v>50</v>
+      </c>
+      <c r="E21" t="n">
         <v>0.307</v>
       </c>
     </row>
@@ -735,12 +800,15 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
+        <v>20</v>
+      </c>
+      <c r="C22" t="n">
         <v>48116</v>
       </c>
-      <c r="C22" t="n">
-        <v>4.5e-05</v>
-      </c>
       <c r="D22" t="n">
+        <v>45</v>
+      </c>
+      <c r="E22" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -749,12 +817,15 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
+        <v>21</v>
+      </c>
+      <c r="C23" t="n">
         <v>50781</v>
       </c>
-      <c r="C23" t="n">
-        <v>5e-05</v>
-      </c>
       <c r="D23" t="n">
+        <v>50</v>
+      </c>
+      <c r="E23" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -763,12 +834,15 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
+        <v>22</v>
+      </c>
+      <c r="C24" t="n">
         <v>53032</v>
       </c>
-      <c r="C24" t="n">
-        <v>5.5e-05</v>
-      </c>
       <c r="D24" t="n">
+        <v>55</v>
+      </c>
+      <c r="E24" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -777,12 +851,15 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
+        <v>23</v>
+      </c>
+      <c r="C25" t="n">
         <v>57416</v>
       </c>
-      <c r="C25" t="n">
-        <v>5.999999999999999e-05</v>
-      </c>
       <c r="D25" t="n">
+        <v>59.99999999999999</v>
+      </c>
+      <c r="E25" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -791,12 +868,15 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
+        <v>24</v>
+      </c>
+      <c r="C26" t="n">
         <v>56611</v>
       </c>
-      <c r="C26" t="n">
-        <v>5.999999999999999e-05</v>
-      </c>
       <c r="D26" t="n">
+        <v>59.99999999999999</v>
+      </c>
+      <c r="E26" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -805,12 +885,15 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
+        <v>25</v>
+      </c>
+      <c r="C27" t="n">
         <v>58553</v>
       </c>
-      <c r="C27" t="n">
-        <v>5.999999999999999e-05</v>
-      </c>
       <c r="D27" t="n">
+        <v>59.99999999999999</v>
+      </c>
+      <c r="E27" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -819,12 +902,15 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
+        <v>26</v>
+      </c>
+      <c r="C28" t="n">
         <v>50784</v>
       </c>
-      <c r="C28" t="n">
-        <v>5e-05</v>
-      </c>
       <c r="D28" t="n">
+        <v>50</v>
+      </c>
+      <c r="E28" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -833,12 +919,15 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
+        <v>27</v>
+      </c>
+      <c r="C29" t="n">
         <v>55491</v>
       </c>
-      <c r="C29" t="n">
-        <v>5.999999999999999e-05</v>
-      </c>
       <c r="D29" t="n">
+        <v>59.99999999999999</v>
+      </c>
+      <c r="E29" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -847,12 +936,15 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
+        <v>28</v>
+      </c>
+      <c r="C30" t="n">
         <v>52405</v>
       </c>
-      <c r="C30" t="n">
-        <v>5.5e-05</v>
-      </c>
       <c r="D30" t="n">
+        <v>55</v>
+      </c>
+      <c r="E30" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -861,12 +953,15 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
+        <v>29</v>
+      </c>
+      <c r="C31" t="n">
         <v>53574</v>
       </c>
-      <c r="C31" t="n">
-        <v>5.5e-05</v>
-      </c>
       <c r="D31" t="n">
+        <v>55</v>
+      </c>
+      <c r="E31" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -875,12 +970,15 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
+        <v>30</v>
+      </c>
+      <c r="C32" t="n">
         <v>53913</v>
       </c>
-      <c r="C32" t="n">
-        <v>5.5e-05</v>
-      </c>
       <c r="D32" t="n">
+        <v>55</v>
+      </c>
+      <c r="E32" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -889,12 +987,15 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
+        <v>31</v>
+      </c>
+      <c r="C33" t="n">
         <v>53434</v>
       </c>
-      <c r="C33" t="n">
-        <v>5.5e-05</v>
-      </c>
       <c r="D33" t="n">
+        <v>55</v>
+      </c>
+      <c r="E33" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -903,12 +1004,15 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
+        <v>32</v>
+      </c>
+      <c r="C34" t="n">
         <v>53641</v>
       </c>
-      <c r="C34" t="n">
-        <v>5.5e-05</v>
-      </c>
       <c r="D34" t="n">
+        <v>55</v>
+      </c>
+      <c r="E34" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -917,12 +1021,15 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
+        <v>33</v>
+      </c>
+      <c r="C35" t="n">
         <v>58358</v>
       </c>
-      <c r="C35" t="n">
-        <v>5.999999999999999e-05</v>
-      </c>
       <c r="D35" t="n">
+        <v>59.99999999999999</v>
+      </c>
+      <c r="E35" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -931,12 +1038,15 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
+        <v>34</v>
+      </c>
+      <c r="C36" t="n">
         <v>51992</v>
       </c>
-      <c r="C36" t="n">
-        <v>5.5e-05</v>
-      </c>
       <c r="D36" t="n">
+        <v>55</v>
+      </c>
+      <c r="E36" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -945,12 +1055,15 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
+        <v>35</v>
+      </c>
+      <c r="C37" t="n">
         <v>59186</v>
       </c>
-      <c r="C37" t="n">
-        <v>6.499999999999999e-05</v>
-      </c>
       <c r="D37" t="n">
+        <v>65</v>
+      </c>
+      <c r="E37" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -959,12 +1072,15 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
+        <v>36</v>
+      </c>
+      <c r="C38" t="n">
         <v>52969</v>
       </c>
-      <c r="C38" t="n">
-        <v>5.5e-05</v>
-      </c>
       <c r="D38" t="n">
+        <v>55</v>
+      </c>
+      <c r="E38" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -973,12 +1089,15 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
+        <v>37</v>
+      </c>
+      <c r="C39" t="n">
         <v>50166</v>
       </c>
-      <c r="C39" t="n">
-        <v>5e-05</v>
-      </c>
       <c r="D39" t="n">
+        <v>50</v>
+      </c>
+      <c r="E39" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -987,12 +1106,15 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
+        <v>38</v>
+      </c>
+      <c r="C40" t="n">
         <v>53044</v>
       </c>
-      <c r="C40" t="n">
-        <v>5.5e-05</v>
-      </c>
       <c r="D40" t="n">
+        <v>55</v>
+      </c>
+      <c r="E40" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -1001,12 +1123,15 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
+        <v>39</v>
+      </c>
+      <c r="C41" t="n">
         <v>53251</v>
       </c>
-      <c r="C41" t="n">
-        <v>5.5e-05</v>
-      </c>
       <c r="D41" t="n">
+        <v>55</v>
+      </c>
+      <c r="E41" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -1015,12 +1140,15 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
+        <v>40</v>
+      </c>
+      <c r="C42" t="n">
         <v>52344</v>
       </c>
-      <c r="C42" t="n">
-        <v>5.5e-05</v>
-      </c>
       <c r="D42" t="n">
+        <v>55</v>
+      </c>
+      <c r="E42" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -1029,12 +1157,15 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
+        <v>41</v>
+      </c>
+      <c r="C43" t="n">
         <v>52071</v>
       </c>
-      <c r="C43" t="n">
-        <v>5.5e-05</v>
-      </c>
       <c r="D43" t="n">
+        <v>55</v>
+      </c>
+      <c r="E43" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -1043,12 +1174,15 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
+        <v>42</v>
+      </c>
+      <c r="C44" t="n">
         <v>51352</v>
       </c>
-      <c r="C44" t="n">
-        <v>5e-05</v>
-      </c>
       <c r="D44" t="n">
+        <v>50</v>
+      </c>
+      <c r="E44" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -1057,12 +1191,15 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
+        <v>43</v>
+      </c>
+      <c r="C45" t="n">
         <v>56541</v>
       </c>
-      <c r="C45" t="n">
-        <v>5.999999999999999e-05</v>
-      </c>
       <c r="D45" t="n">
+        <v>59.99999999999999</v>
+      </c>
+      <c r="E45" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -1071,12 +1208,15 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
+        <v>44</v>
+      </c>
+      <c r="C46" t="n">
         <v>52824</v>
       </c>
-      <c r="C46" t="n">
-        <v>5.5e-05</v>
-      </c>
       <c r="D46" t="n">
+        <v>55</v>
+      </c>
+      <c r="E46" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -1085,12 +1225,15 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
+        <v>45</v>
+      </c>
+      <c r="C47" t="n">
         <v>50351</v>
       </c>
-      <c r="C47" t="n">
-        <v>5e-05</v>
-      </c>
       <c r="D47" t="n">
+        <v>50</v>
+      </c>
+      <c r="E47" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -1099,12 +1242,15 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
+        <v>46</v>
+      </c>
+      <c r="C48" t="n">
         <v>53642</v>
       </c>
-      <c r="C48" t="n">
-        <v>5.5e-05</v>
-      </c>
       <c r="D48" t="n">
+        <v>55</v>
+      </c>
+      <c r="E48" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -1113,12 +1259,15 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
+        <v>47</v>
+      </c>
+      <c r="C49" t="n">
         <v>50530</v>
       </c>
-      <c r="C49" t="n">
-        <v>5e-05</v>
-      </c>
       <c r="D49" t="n">
+        <v>50</v>
+      </c>
+      <c r="E49" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -1127,12 +1276,15 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
+        <v>48</v>
+      </c>
+      <c r="C50" t="n">
         <v>47151</v>
       </c>
-      <c r="C50" t="n">
-        <v>4.5e-05</v>
-      </c>
       <c r="D50" t="n">
+        <v>45</v>
+      </c>
+      <c r="E50" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -1141,12 +1293,15 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
+        <v>49</v>
+      </c>
+      <c r="C51" t="n">
         <v>53052</v>
       </c>
-      <c r="C51" t="n">
-        <v>5.5e-05</v>
-      </c>
       <c r="D51" t="n">
+        <v>55</v>
+      </c>
+      <c r="E51" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -1155,12 +1310,15 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
+        <v>50</v>
+      </c>
+      <c r="C52" t="n">
         <v>52202</v>
       </c>
-      <c r="C52" t="n">
-        <v>5.5e-05</v>
-      </c>
       <c r="D52" t="n">
+        <v>55</v>
+      </c>
+      <c r="E52" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -1169,12 +1327,15 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
+        <v>51</v>
+      </c>
+      <c r="C53" t="n">
         <v>52204</v>
       </c>
-      <c r="C53" t="n">
-        <v>5.5e-05</v>
-      </c>
       <c r="D53" t="n">
+        <v>55</v>
+      </c>
+      <c r="E53" t="n">
         <v>0.316</v>
       </c>
     </row>
@@ -1183,12 +1344,15 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
+        <v>52</v>
+      </c>
+      <c r="C54" t="n">
         <v>54509</v>
       </c>
-      <c r="C54" t="n">
-        <v>5.5e-05</v>
-      </c>
       <c r="D54" t="n">
+        <v>55</v>
+      </c>
+      <c r="E54" t="n">
         <v>0.31</v>
       </c>
     </row>
@@ -1197,12 +1361,15 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
+        <v>53</v>
+      </c>
+      <c r="C55" t="n">
         <v>54985</v>
       </c>
-      <c r="C55" t="n">
-        <v>5.5e-05</v>
-      </c>
       <c r="D55" t="n">
+        <v>55</v>
+      </c>
+      <c r="E55" t="n">
         <v>0.31</v>
       </c>
     </row>
@@ -1211,12 +1378,15 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
+        <v>54</v>
+      </c>
+      <c r="C56" t="n">
         <v>53786</v>
       </c>
-      <c r="C56" t="n">
-        <v>5.5e-05</v>
-      </c>
       <c r="D56" t="n">
+        <v>55</v>
+      </c>
+      <c r="E56" t="n">
         <v>0.31</v>
       </c>
     </row>
@@ -1225,12 +1395,15 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
+        <v>55</v>
+      </c>
+      <c r="C57" t="n">
         <v>51218</v>
       </c>
-      <c r="C57" t="n">
-        <v>5e-05</v>
-      </c>
       <c r="D57" t="n">
+        <v>50</v>
+      </c>
+      <c r="E57" t="n">
         <v>0.31</v>
       </c>
     </row>
@@ -1239,12 +1412,15 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
+        <v>56</v>
+      </c>
+      <c r="C58" t="n">
         <v>54522</v>
       </c>
-      <c r="C58" t="n">
-        <v>5.5e-05</v>
-      </c>
       <c r="D58" t="n">
+        <v>55</v>
+      </c>
+      <c r="E58" t="n">
         <v>0.31</v>
       </c>
     </row>
@@ -1253,12 +1429,15 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
+        <v>57</v>
+      </c>
+      <c r="C59" t="n">
         <v>51023</v>
       </c>
-      <c r="C59" t="n">
-        <v>5e-05</v>
-      </c>
       <c r="D59" t="n">
+        <v>50</v>
+      </c>
+      <c r="E59" t="n">
         <v>0.31</v>
       </c>
     </row>
@@ -1267,12 +1446,15 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
+        <v>58</v>
+      </c>
+      <c r="C60" t="n">
         <v>56169</v>
       </c>
-      <c r="C60" t="n">
-        <v>5.999999999999999e-05</v>
-      </c>
       <c r="D60" t="n">
+        <v>59.99999999999999</v>
+      </c>
+      <c r="E60" t="n">
         <v>0.31</v>
       </c>
     </row>
@@ -1281,12 +1463,15 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
+        <v>59</v>
+      </c>
+      <c r="C61" t="n">
         <v>57116</v>
       </c>
-      <c r="C61" t="n">
-        <v>5.999999999999999e-05</v>
-      </c>
       <c r="D61" t="n">
+        <v>59.99999999999999</v>
+      </c>
+      <c r="E61" t="n">
         <v>0.31</v>
       </c>
     </row>
@@ -1295,12 +1480,15 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
+        <v>60</v>
+      </c>
+      <c r="C62" t="n">
         <v>55717</v>
       </c>
-      <c r="C62" t="n">
-        <v>5.5e-05</v>
-      </c>
       <c r="D62" t="n">
+        <v>55</v>
+      </c>
+      <c r="E62" t="n">
         <v>0.31</v>
       </c>
     </row>
@@ -1309,12 +1497,15 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
+        <v>61</v>
+      </c>
+      <c r="C63" t="n">
         <v>47487</v>
       </c>
-      <c r="C63" t="n">
-        <v>4.5e-05</v>
-      </c>
       <c r="D63" t="n">
+        <v>45</v>
+      </c>
+      <c r="E63" t="n">
         <v>0.31</v>
       </c>
     </row>
@@ -1323,12 +1514,15 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
+        <v>62</v>
+      </c>
+      <c r="C64" t="n">
         <v>52075</v>
       </c>
-      <c r="C64" t="n">
-        <v>5e-05</v>
-      </c>
       <c r="D64" t="n">
+        <v>50</v>
+      </c>
+      <c r="E64" t="n">
         <v>0.31</v>
       </c>
     </row>
@@ -1337,12 +1531,15 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
+        <v>63</v>
+      </c>
+      <c r="C65" t="n">
         <v>55600</v>
       </c>
-      <c r="C65" t="n">
-        <v>5.5e-05</v>
-      </c>
       <c r="D65" t="n">
+        <v>55</v>
+      </c>
+      <c r="E65" t="n">
         <v>0.297</v>
       </c>
     </row>
@@ -1351,12 +1548,15 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
+        <v>64</v>
+      </c>
+      <c r="C66" t="n">
         <v>61411</v>
       </c>
-      <c r="C66" t="n">
-        <v>5.999999999999999e-05</v>
-      </c>
       <c r="D66" t="n">
+        <v>59.99999999999999</v>
+      </c>
+      <c r="E66" t="n">
         <v>0.297</v>
       </c>
     </row>
@@ -1365,12 +1565,15 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
+        <v>65</v>
+      </c>
+      <c r="C67" t="n">
         <v>47804</v>
       </c>
-      <c r="C67" t="n">
-        <v>4e-05</v>
-      </c>
       <c r="D67" t="n">
+        <v>40</v>
+      </c>
+      <c r="E67" t="n">
         <v>0.297</v>
       </c>
     </row>
@@ -1379,12 +1582,15 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
+        <v>66</v>
+      </c>
+      <c r="C68" t="n">
         <v>55195</v>
       </c>
-      <c r="C68" t="n">
-        <v>5.5e-05</v>
-      </c>
       <c r="D68" t="n">
+        <v>55</v>
+      </c>
+      <c r="E68" t="n">
         <v>0.297</v>
       </c>
     </row>
@@ -1393,12 +1599,15 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
+        <v>67</v>
+      </c>
+      <c r="C69" t="n">
         <v>54198</v>
       </c>
-      <c r="C69" t="n">
-        <v>5e-05</v>
-      </c>
       <c r="D69" t="n">
+        <v>50</v>
+      </c>
+      <c r="E69" t="n">
         <v>0.297</v>
       </c>
     </row>
@@ -1407,12 +1616,15 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
+        <v>68</v>
+      </c>
+      <c r="C70" t="n">
         <v>56945</v>
       </c>
-      <c r="C70" t="n">
-        <v>5.5e-05</v>
-      </c>
       <c r="D70" t="n">
+        <v>55</v>
+      </c>
+      <c r="E70" t="n">
         <v>0.297</v>
       </c>
     </row>
@@ -1421,12 +1633,15 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
+        <v>69</v>
+      </c>
+      <c r="C71" t="n">
         <v>65337</v>
       </c>
-      <c r="C71" t="n">
-        <v>6.499999999999999e-05</v>
-      </c>
       <c r="D71" t="n">
+        <v>65</v>
+      </c>
+      <c r="E71" t="n">
         <v>0.297</v>
       </c>
     </row>
@@ -1435,12 +1650,15 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
+        <v>70</v>
+      </c>
+      <c r="C72" t="n">
         <v>61250</v>
       </c>
-      <c r="C72" t="n">
-        <v>5.999999999999999e-05</v>
-      </c>
       <c r="D72" t="n">
+        <v>59.99999999999999</v>
+      </c>
+      <c r="E72" t="n">
         <v>0.297</v>
       </c>
     </row>
@@ -1449,12 +1667,15 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
+        <v>71</v>
+      </c>
+      <c r="C73" t="n">
         <v>52366</v>
       </c>
-      <c r="C73" t="n">
-        <v>4.5e-05</v>
-      </c>
       <c r="D73" t="n">
+        <v>45</v>
+      </c>
+      <c r="E73" t="n">
         <v>0.297</v>
       </c>
     </row>
@@ -1463,12 +1684,15 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
+        <v>72</v>
+      </c>
+      <c r="C74" t="n">
         <v>53721</v>
       </c>
-      <c r="C74" t="n">
-        <v>5e-05</v>
-      </c>
       <c r="D74" t="n">
+        <v>50</v>
+      </c>
+      <c r="E74" t="n">
         <v>0.297</v>
       </c>
     </row>
@@ -1477,12 +1701,15 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
+        <v>73</v>
+      </c>
+      <c r="C75" t="n">
         <v>59053</v>
       </c>
-      <c r="C75" t="n">
-        <v>5.5e-05</v>
-      </c>
       <c r="D75" t="n">
+        <v>55</v>
+      </c>
+      <c r="E75" t="n">
         <v>0.297</v>
       </c>
     </row>
@@ -1491,12 +1718,15 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
+        <v>74</v>
+      </c>
+      <c r="C76" t="n">
         <v>58843</v>
       </c>
-      <c r="C76" t="n">
-        <v>5.5e-05</v>
-      </c>
       <c r="D76" t="n">
+        <v>55</v>
+      </c>
+      <c r="E76" t="n">
         <v>0.297</v>
       </c>
     </row>
@@ -1505,12 +1735,15 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
+        <v>75</v>
+      </c>
+      <c r="C77" t="n">
         <v>52728</v>
       </c>
-      <c r="C77" t="n">
-        <v>4.5e-05</v>
-      </c>
       <c r="D77" t="n">
+        <v>45</v>
+      </c>
+      <c r="E77" t="n">
         <v>0.297</v>
       </c>
     </row>
@@ -1519,12 +1752,15 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
+        <v>76</v>
+      </c>
+      <c r="C78" t="n">
         <v>55748</v>
       </c>
-      <c r="C78" t="n">
-        <v>5.5e-05</v>
-      </c>
       <c r="D78" t="n">
+        <v>55</v>
+      </c>
+      <c r="E78" t="n">
         <v>0.297</v>
       </c>
     </row>
@@ -1533,12 +1769,15 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
+        <v>77</v>
+      </c>
+      <c r="C79" t="n">
         <v>53157</v>
       </c>
-      <c r="C79" t="n">
-        <v>5e-05</v>
-      </c>
       <c r="D79" t="n">
+        <v>50</v>
+      </c>
+      <c r="E79" t="n">
         <v>0.297</v>
       </c>
     </row>
@@ -1547,12 +1786,15 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
+        <v>78</v>
+      </c>
+      <c r="C80" t="n">
         <v>55333</v>
       </c>
-      <c r="C80" t="n">
-        <v>5e-05</v>
-      </c>
       <c r="D80" t="n">
+        <v>50</v>
+      </c>
+      <c r="E80" t="n">
         <v>0.297</v>
       </c>
     </row>
@@ -1561,12 +1803,15 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
+        <v>79</v>
+      </c>
+      <c r="C81" t="n">
         <v>54478</v>
       </c>
-      <c r="C81" t="n">
-        <v>5e-05</v>
-      </c>
       <c r="D81" t="n">
+        <v>50</v>
+      </c>
+      <c r="E81" t="n">
         <v>0.297</v>
       </c>
     </row>

</xml_diff>